<commit_message>
* .PDF also included * New Customer added
</commit_message>
<xml_diff>
--- a/res/keywords.xlsx
+++ b/res/keywords.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan\IdeaProjects\ScanManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse\workspace-sts-3.7.3.RELEASE\ScanManager\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BACAF22-9489-4F48-AE83-30F3EEF8D3F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B64155-C5CB-4A9F-A72F-76D1DFACDB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19752" yWindow="1416" windowWidth="19212" windowHeight="15264" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37080" yWindow="-2016" windowWidth="22380" windowHeight="14712" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="File-Keys" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
   <si>
     <t>Telenet</t>
   </si>
@@ -213,6 +213,12 @@
   </si>
   <si>
     <t>(0543361732)</t>
+  </si>
+  <si>
+    <t>GeraardsbergseBandencentrale</t>
+  </si>
+  <si>
+    <t>BE0456623540</t>
   </si>
 </sst>
 </file>
@@ -248,9 +254,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -534,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -592,7 +597,7 @@
       <c r="B4" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>58</v>
       </c>
     </row>
@@ -619,7 +624,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
@@ -663,7 +668,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
@@ -801,6 +806,17 @@
       </c>
       <c r="D22" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Robbshop added in xls
</commit_message>
<xml_diff>
--- a/res/keywords.xlsx
+++ b/res/keywords.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse\workspace-sts-3.7.3.RELEASE\ScanManager\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B64155-C5CB-4A9F-A72F-76D1DFACDB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3EFEC09A-8FE6-4B37-B888-926FD3E533F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37080" yWindow="-2016" windowWidth="22380" windowHeight="14712" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-46188" yWindow="-8508" windowWidth="46296" windowHeight="25680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="File-Keys" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
   <si>
     <t>Telenet</t>
   </si>
@@ -219,6 +219,12 @@
   </si>
   <si>
     <t>BE0456623540</t>
+  </si>
+  <si>
+    <t>ROBBshop</t>
+  </si>
+  <si>
+    <t>Factuurnr</t>
   </si>
 </sst>
 </file>
@@ -539,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -819,6 +825,17 @@
         <v>28</v>
       </c>
     </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Billit, Carglass added, .idea added to .gitignore
</commit_message>
<xml_diff>
--- a/res/keywords.xlsx
+++ b/res/keywords.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse\ScanManager\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3EFEC09A-8FE6-4B37-B888-926FD3E533F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD16D0E6-9ED3-4351-9EE6-0BF582286AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-46188" yWindow="-8508" windowWidth="46296" windowHeight="25680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32736" yWindow="-4428" windowWidth="27708" windowHeight="16824" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="File-Keys" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
   <si>
     <t>Telenet</t>
   </si>
@@ -225,6 +225,15 @@
   </si>
   <si>
     <t>Factuurnr</t>
+  </si>
+  <si>
+    <t>Carglass</t>
+  </si>
+  <si>
+    <t>Billit</t>
+  </si>
+  <si>
+    <t>BILLIT</t>
   </si>
 </sst>
 </file>
@@ -545,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -836,6 +845,28 @@
         <v>62</v>
       </c>
     </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>